<commit_message>
added xlsx files (#1)
</commit_message>
<xml_diff>
--- a/03_Planning/ProductBurndown.xlsx
+++ b/03_Planning/ProductBurndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\guideo\03_Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DAE6D1-FF8E-43D7-9717-76DD7489371E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A84499-503C-47CF-93FC-126CACEEB1CD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1126,8 +1126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N38" sqref="N38"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3072,7 +3072,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A10" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>